<commit_message>
My callendar with password 123
</commit_message>
<xml_diff>
--- a/My Calendar.xlsx
+++ b/My Calendar.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EXCEL\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{28418068-0651-41E5-A6AA-42A3D3EF13BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29B123DC-FAE6-48E8-BBCF-ED4B8C99277F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -522,167 +522,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thick">
         <color rgb="FF000000"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thick">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="thick">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thick">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -724,167 +567,336 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color theme="1"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1310,1346 +1322,1352 @@
   </sheetPr>
   <dimension ref="A1:M996"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" defaultGridColor="0" topLeftCell="B1" colorId="9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1 A1 E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" customWidth="1"/>
-    <col min="3" max="9" width="13.5703125" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21" customWidth="1"/>
-    <col min="12" max="12" width="20.85546875" customWidth="1"/>
-    <col min="13" max="13" width="15.7109375" customWidth="1"/>
-    <col min="14" max="27" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" style="3" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="3" customWidth="1"/>
+    <col min="3" max="9" width="13.5703125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21" style="3" customWidth="1"/>
+    <col min="12" max="12" width="20.85546875" style="3" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" style="3" customWidth="1"/>
+    <col min="14" max="27" width="8.7109375" style="3" customWidth="1"/>
+    <col min="28" max="16384" width="14.42578125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="28.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="9">
+      <c r="A1" s="1">
         <f>IF(E1 = "Fev", IF( MOD(I1, 4) = 0, IF( MOD(I1, 100) = 0, IF( MOD(I1, 400) = 0, 1,), 1),),)</f>
         <v>1</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="57" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="58"/>
-      <c r="E1" s="59" t="s">
+      <c r="D1" s="13"/>
+      <c r="E1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="60"/>
-      <c r="G1" s="61" t="s">
+      <c r="F1" s="15"/>
+      <c r="G1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="61"/>
-      <c r="I1" s="62">
+      <c r="H1" s="16"/>
+      <c r="I1" s="17">
         <v>2020</v>
       </c>
-      <c r="J1" s="16"/>
-      <c r="K1" s="9"/>
-      <c r="M1" s="9"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="1"/>
+      <c r="M1" s="1"/>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="str">
+      <c r="A2" s="2" t="str">
         <f>CONCATENATE("01", "/", $E$1, "/", $I$1)</f>
         <v>01/Fev/2020</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="M2" s="9"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="M2" s="1"/>
     </row>
     <row r="3" spans="1:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C3" s="7" t="str">
+      <c r="C3" s="19" t="str">
         <f ca="1">"DIA: "&amp;DAY(TODAY())</f>
-        <v>DIA: 2</v>
-      </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="13" t="str">
+        <v>DIA: 4</v>
+      </c>
+      <c r="D3" s="20"/>
+      <c r="E3" s="21" t="str">
         <f ca="1">"MÊS DE "&amp;UPPER(TEXT(TODAY(), "mmmm"))</f>
         <v>MÊS DE MAIO</v>
       </c>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="11" t="str">
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="23" t="str">
         <f ca="1">"ANO: "&amp;YEAR(TODAY())</f>
         <v>ANO: 2019</v>
       </c>
-      <c r="I3" s="12"/>
-      <c r="M3" s="9"/>
+      <c r="I3" s="22"/>
+      <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:13" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="2" t="s">
+      <c r="B4" s="7"/>
+      <c r="C4" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="9"/>
+      <c r="M4" s="1"/>
     </row>
     <row r="5" spans="1:13" ht="52.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="21" t="str">
+      <c r="B5" s="8"/>
+      <c r="C5" s="35" t="str">
         <f>IF( TEXT( $A$2, "ddd" ) = C$4,  1,  "" )</f>
         <v/>
       </c>
-      <c r="D5" s="22" t="str">
-        <f>IF( TEXT( $A$2, "ddd" ) = D$4, 1, IF( C$5 &lt;&gt; "", C$5 + 1, "" ))</f>
+      <c r="D5" s="36" t="str">
+        <f t="shared" ref="D5:I5" si="0">IF( TEXT( $A$2, "ddd" ) = D$4, 1, IF( C$5 &lt;&gt; "", C$5 + 1, "" ))</f>
         <v/>
       </c>
-      <c r="E5" s="23" t="str">
-        <f>IF( TEXT( $A$2, "ddd" ) = E$4, 1, IF( D$5 &lt;&gt; "", D$5 + 1, "" ))</f>
+      <c r="E5" s="37" t="str">
+        <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F5" s="24" t="str">
-        <f>IF( TEXT( $A$2, "ddd" ) = F$4, 1, IF( E$5 &lt;&gt; "", E$5 + 1, "" ))</f>
+      <c r="F5" s="38" t="str">
+        <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G5" s="25" t="str">
+      <c r="G5" s="39" t="str">
         <f>IF( TEXT( $A$2, "ddd" ) = G$4, 1, IF( F$5 &lt;&gt; "", F$5 + 1, "" ))</f>
         <v/>
       </c>
-      <c r="H5" s="26" t="str">
-        <f>IF( TEXT( $A$2, "ddd" ) = H$4, 1, IF( G$5 &lt;&gt; "", G$5 + 1, "" ))</f>
+      <c r="H5" s="40" t="str">
+        <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I5" s="27">
-        <f>IF( TEXT( $A$2, "ddd" ) = I$4, 1, IF( H$5 &lt;&gt; "", H$5 + 1, "" ))</f>
+      <c r="I5" s="41">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="M5" s="9"/>
+      <c r="J5" s="27"/>
+      <c r="M5" s="1"/>
     </row>
     <row r="6" spans="1:13" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="28">
+      <c r="B6" s="9"/>
+      <c r="C6" s="56">
         <f>IFERROR(IF( OR( $E$1 = "Abr",  $E$1 = "Jun", $E$1 = "Set", $E$1 = "Nov"), IF(I5&gt;29, "", I5+1), IF( $E$1 = "Fev", IF( I5&gt;27 + $A$1, "", I5+1), IF(I5&gt;30, "", I5+1))), "")</f>
         <v>2</v>
       </c>
-      <c r="D6" s="29">
-        <f>IFERROR(IF( OR( $E$1 = "Abr",  $E$1 = "Jun", $E$1 = "Set", $E$1 = "Nov"), IF(C6&gt;29, "", C6+1), IF( $E$1 = "Fev", IF( C6&gt;27+$A$1, "", C6+1), IF(C6&gt;30, "", C6+1))), "")</f>
+      <c r="D6" s="30">
+        <f t="shared" ref="D6:I10" si="1">IFERROR(IF( OR( $E$1 = "Abr",  $E$1 = "Jun", $E$1 = "Set", $E$1 = "Nov"), IF(C6&gt;29, "", C6+1), IF( $E$1 = "Fev", IF( C6&gt;27+$A$1, "", C6+1), IF(C6&gt;30, "", C6+1))), "")</f>
         <v>3</v>
       </c>
-      <c r="E6" s="30">
-        <f>IFERROR(IF( OR( $E$1 = "Abr",  $E$1 = "Jun", $E$1 = "Set", $E$1 = "Nov"), IF(D6&gt;29, "", D6+1), IF( $E$1 = "Fev", IF( D6&gt;27+$A$1, "", D6+1), IF(D6&gt;30, "", D6+1))), "")</f>
+      <c r="E6" s="31">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="F6" s="31">
-        <f>IFERROR(IF( OR( $E$1 = "Abr",  $E$1 = "Jun", $E$1 = "Set", $E$1 = "Nov"), IF(E6&gt;29, "", E6+1), IF( $E$1 = "Fev", IF( E6&gt;27+$A$1, "", E6+1), IF(E6&gt;30, "", E6+1))), "")</f>
+      <c r="F6" s="32">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="G6" s="32">
-        <f>IFERROR(IF( OR( $E$1 = "Abr",  $E$1 = "Jun", $E$1 = "Set", $E$1 = "Nov"), IF(F6&gt;29, "", F6+1), IF( $E$1 = "Fev", IF( F6&gt;27+$A$1, "", F6+1), IF(F6&gt;30, "", F6+1))), "")</f>
+      <c r="G6" s="33">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="H6" s="33">
-        <f>IFERROR(IF( OR( $E$1 = "Abr",  $E$1 = "Jun", $E$1 = "Set", $E$1 = "Nov"), IF(G6&gt;29, "", G6+1), IF( $E$1 = "Fev", IF( G6&gt;27+$A$1, "", G6+1), IF(G6&gt;30, "", G6+1))), "")</f>
+      <c r="H6" s="34">
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="I6" s="34">
-        <f>IFERROR(IF( OR( $E$1 = "Abr",  $E$1 = "Jun", $E$1 = "Set", $E$1 = "Nov"), IF(H6&gt;29, "", H6+1), IF( $E$1 = "Fev", IF( H6&gt;27+$A$1, "", H6+1), IF(H6&gt;30, "", H6+1))), "")</f>
+      <c r="I6" s="57">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="J6" s="1"/>
-      <c r="M6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="M6" s="1"/>
     </row>
     <row r="7" spans="1:13" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="35">
+      <c r="B7" s="8"/>
+      <c r="C7" s="49">
         <f>IFERROR(IF( OR( $E$1 = "Abr",  $E$1 = "Jun", $E$1 = "Set", $E$1 = "Nov"), IF(I6&gt;29, "", I6+1), IF( $E$1 = "Fev", IF( I6&gt;27 + $A$1, "", I6+1), IF(I6&gt;30, "", I6+1))), "")</f>
         <v>9</v>
       </c>
-      <c r="D7" s="36">
-        <f>IFERROR(IF( OR( $E$1 = "Abr",  $E$1 = "Jun", $E$1 = "Set", $E$1 = "Nov"), IF(C7&gt;29, "", C7+1), IF( $E$1 = "Fev", IF( C7&gt;27+$A$1, "", C7+1), IF(C7&gt;30, "", C7+1))), "")</f>
+      <c r="D7" s="50">
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="E7" s="37">
-        <f>IFERROR(IF( OR( $E$1 = "Abr",  $E$1 = "Jun", $E$1 = "Set", $E$1 = "Nov"), IF(D7&gt;29, "", D7+1), IF( $E$1 = "Fev", IF( D7&gt;27+$A$1, "", D7+1), IF(D7&gt;30, "", D7+1))), "")</f>
+      <c r="E7" s="51">
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="F7" s="24">
-        <f>IFERROR(IF( OR( $E$1 = "Abr",  $E$1 = "Jun", $E$1 = "Set", $E$1 = "Nov"), IF(E7&gt;29, "", E7+1), IF( $E$1 = "Fev", IF( E7&gt;27+$A$1, "", E7+1), IF(E7&gt;30, "", E7+1))), "")</f>
+      <c r="F7" s="52">
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="G7" s="38">
-        <f>IFERROR(IF( OR( $E$1 = "Abr",  $E$1 = "Jun", $E$1 = "Set", $E$1 = "Nov"), IF(F7&gt;29, "", F7+1), IF( $E$1 = "Fev", IF( F7&gt;27+$A$1, "", F7+1), IF(F7&gt;30, "", F7+1))), "")</f>
+      <c r="G7" s="53">
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="H7" s="39">
-        <f>IFERROR(IF( OR( $E$1 = "Abr",  $E$1 = "Jun", $E$1 = "Set", $E$1 = "Nov"), IF(G7&gt;29, "", G7+1), IF( $E$1 = "Fev", IF( G7&gt;27+$A$1, "", G7+1), IF(G7&gt;30, "", G7+1))), "")</f>
+      <c r="H7" s="54">
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="I7" s="40">
-        <f>IFERROR(IF( OR( $E$1 = "Abr",  $E$1 = "Jun", $E$1 = "Set", $E$1 = "Nov"), IF(H7&gt;29, "", H7+1), IF( $E$1 = "Fev", IF( H7&gt;27+$A$1, "", H7+1), IF(H7&gt;30, "", H7+1))), "")</f>
+      <c r="I7" s="55">
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="M7" s="9"/>
+      <c r="J7" s="4"/>
+      <c r="M7" s="1"/>
     </row>
     <row r="8" spans="1:13" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="41">
+      <c r="B8" s="28"/>
+      <c r="C8" s="56">
         <f>IFERROR(IF( OR( $E$1 = "Abr",  $E$1 = "Jun", $E$1 = "Set", $E$1 = "Nov"), IF(I7&gt;29, "", I7+1), IF( $E$1 = "Fev", IF( I7&gt;27 + $A$1, "", I7+1), IF(I7&gt;30, "", I7+1))), "")</f>
         <v>16</v>
       </c>
-      <c r="D8" s="42">
-        <f>IFERROR(IF( OR( $E$1 = "Abr",  $E$1 = "Jun", $E$1 = "Set", $E$1 = "Nov"), IF(C8&gt;29, "", C8+1), IF( $E$1 = "Fev", IF( C8&gt;27+$A$1, "", C8+1), IF(C8&gt;30, "", C8+1))), "")</f>
+      <c r="D8" s="30">
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="E8" s="43">
-        <f>IFERROR(IF( OR( $E$1 = "Abr",  $E$1 = "Jun", $E$1 = "Set", $E$1 = "Nov"), IF(D8&gt;29, "", D8+1), IF( $E$1 = "Fev", IF( D8&gt;27+$A$1, "", D8+1), IF(D8&gt;30, "", D8+1))), "")</f>
+      <c r="E8" s="31">
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="F8" s="20">
-        <f>IFERROR(IF( OR( $E$1 = "Abr",  $E$1 = "Jun", $E$1 = "Set", $E$1 = "Nov"), IF(E8&gt;29, "", E8+1), IF( $E$1 = "Fev", IF( E8&gt;27+$A$1, "", E8+1), IF(E8&gt;30, "", E8+1))), "")</f>
+      <c r="F8" s="32">
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="G8" s="44">
-        <f>IFERROR(IF( OR( $E$1 = "Abr",  $E$1 = "Jun", $E$1 = "Set", $E$1 = "Nov"), IF(F8&gt;29, "", F8+1), IF( $E$1 = "Fev", IF( F8&gt;27+$A$1, "", F8+1), IF(F8&gt;30, "", F8+1))), "")</f>
+      <c r="G8" s="33">
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="H8" s="45">
-        <f>IFERROR(IF( OR( $E$1 = "Abr",  $E$1 = "Jun", $E$1 = "Set", $E$1 = "Nov"), IF(G8&gt;29, "", G8+1), IF( $E$1 = "Fev", IF( G8&gt;27+$A$1, "", G8+1), IF(G8&gt;30, "", G8+1))), "")</f>
+      <c r="H8" s="34">
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="I8" s="46">
-        <f>IFERROR(IF( OR( $E$1 = "Abr",  $E$1 = "Jun", $E$1 = "Set", $E$1 = "Nov"), IF(H8&gt;29, "", H8+1), IF( $E$1 = "Fev", IF( H8&gt;27+$A$1, "", H8+1), IF(H8&gt;30, "", H8+1))), "")</f>
+      <c r="I8" s="57">
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="J8" s="15"/>
-      <c r="M8" s="9"/>
+      <c r="J8" s="5"/>
+      <c r="M8" s="1"/>
     </row>
     <row r="9" spans="1:13" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="47">
+      <c r="B9" s="29"/>
+      <c r="C9" s="58">
         <f>IFERROR(IF( OR( $E$1 = "Abr",  $E$1 = "Jun", $E$1 = "Set", $E$1 = "Nov"), IF(I8&gt;29, "", I8+1), IF( $E$1 = "Fev", IF( I8&gt;27 + $A$1, "", I8+1), IF(I8&gt;30, "", I8+1))), "")</f>
         <v>23</v>
       </c>
-      <c r="D9" s="29">
-        <f>IFERROR(IF( OR( $E$1 = "Abr",  $E$1 = "Jun", $E$1 = "Set", $E$1 = "Nov"), IF(C9&gt;29, "", C9+1), IF( $E$1 = "Fev", IF( C9&gt;27+$A$1, "", C9+1), IF(C9&gt;30, "", C9+1))), "")</f>
+      <c r="D9" s="50">
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="E9" s="30">
-        <f>IFERROR(IF( OR( $E$1 = "Abr",  $E$1 = "Jun", $E$1 = "Set", $E$1 = "Nov"), IF(D9&gt;29, "", D9+1), IF( $E$1 = "Fev", IF( D9&gt;27+$A$1, "", D9+1), IF(D9&gt;30, "", D9+1))), "")</f>
+      <c r="E9" s="51">
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="F9" s="24">
-        <f>IFERROR(IF( OR( $E$1 = "Abr",  $E$1 = "Jun", $E$1 = "Set", $E$1 = "Nov"), IF(E9&gt;29, "", E9+1), IF( $E$1 = "Fev", IF( E9&gt;27+$A$1, "", E9+1), IF(E9&gt;30, "", E9+1))), "")</f>
+      <c r="F9" s="52">
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="G9" s="32">
-        <f>IFERROR(IF( OR( $E$1 = "Abr",  $E$1 = "Jun", $E$1 = "Set", $E$1 = "Nov"), IF(F9&gt;29, "", F9+1), IF( $E$1 = "Fev", IF( F9&gt;27+$A$1, "", F9+1), IF(F9&gt;30, "", F9+1))), "")</f>
+      <c r="G9" s="53">
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="H9" s="33">
-        <f>IFERROR(IF( OR( $E$1 = "Abr",  $E$1 = "Jun", $E$1 = "Set", $E$1 = "Nov"), IF(G9&gt;29, "", G9+1), IF( $E$1 = "Fev", IF( G9&gt;27+$A$1, "", G9+1), IF(G9&gt;30, "", G9+1))), "")</f>
+      <c r="H9" s="54">
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="I9" s="48">
-        <f>IFERROR(IF( OR( $E$1 = "Abr",  $E$1 = "Jun", $E$1 = "Set", $E$1 = "Nov"), IF(H9&gt;29, "", H9+1), IF( $E$1 = "Fev", IF( H9&gt;27+$A$1, "", H9+1), IF(H9&gt;30, "", H9+1))), "")</f>
+      <c r="I9" s="55">
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="J9" s="19"/>
+      <c r="J9" s="4"/>
     </row>
     <row r="10" spans="1:13" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="49" t="str">
+      <c r="C10" s="42" t="str">
         <f>IFERROR(IF( OR( $E$1 = "Abr",  $E$1 = "Jun", $E$1 = "Set", $E$1 = "Nov"), IF(I9&gt;29, "", I9+1), IF( $E$1 = "Fev", IF( I9&gt;27 + $A$1, "", I9+1), IF(I9&gt;30, "", I9+1))), "")</f>
         <v/>
       </c>
-      <c r="D10" s="50" t="str">
-        <f>IFERROR(IF( OR( $E$1 = "Abr",  $E$1 = "Jun", $E$1 = "Set", $E$1 = "Nov"), IF(C10&gt;29, "", C10+1), IF( $E$1 = "Fev", IF( C10&gt;27+$A$1, "", C10+1), IF(C10&gt;30, "", C10+1))), "")</f>
+      <c r="D10" s="43" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E10" s="51" t="str">
-        <f>IFERROR(IF( OR( $E$1 = "Abr",  $E$1 = "Jun", $E$1 = "Set", $E$1 = "Nov"), IF(D10&gt;29, "", D10+1), IF( $E$1 = "Fev", IF( D10&gt;27+$A$1, "", D10+1), IF(D10&gt;30, "", D10+1))), "")</f>
+      <c r="E10" s="44" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F10" s="52" t="str">
-        <f>IFERROR(IF( OR( $E$1 = "Abr",  $E$1 = "Jun", $E$1 = "Set", $E$1 = "Nov"), IF(E10&gt;29, "", E10+1), IF( $E$1 = "Fev", IF( E10&gt;27+$A$1, "", E10+1), IF(E10&gt;30, "", E10+1))), "")</f>
+      <c r="F10" s="45" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G10" s="53" t="str">
-        <f>IFERROR(IF( OR( $E$1 = "Abr",  $E$1 = "Jun", $E$1 = "Set", $E$1 = "Nov"), IF(F10&gt;29, "", F10+1), IF( $E$1 = "Fev", IF( F10&gt;27+$A$1, "", F10+1), IF(F10&gt;30, "", F10+1))), "")</f>
+      <c r="G10" s="46" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="H10" s="54" t="str">
-        <f>IFERROR(IF( OR( $E$1 = "Abr",  $E$1 = "Jun", $E$1 = "Set", $E$1 = "Nov"), IF(G10&gt;29, "", G10+1), IF( $E$1 = "Fev", IF( G10&gt;27+$A$1, "", G10+1), IF(G10&gt;30, "", G10+1))), "")</f>
+      <c r="H10" s="47" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="I10" s="55" t="str">
-        <f>IFERROR(IF( OR( $E$1 = "Abr",  $E$1 = "Jun", $E$1 = "Set", $E$1 = "Nov"), IF(H10&gt;29, "", H10+1), IF( $E$1 = "Fev", IF( H10&gt;27+$A$1, "", H10+1), IF(H10&gt;30, "", H10+1))), "")</f>
+      <c r="I10" s="48" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="11" spans="1:13" ht="17.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="10" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="10" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="10" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="10" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="10" t="s">
         <v>20</v>
       </c>
     </row>
+    <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+    </row>
     <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="A17" s="11">
         <v>1900</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="A18" s="11">
         <v>1901</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="A19" s="11">
         <v>1902</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="A20" s="11">
         <v>1903</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="A21" s="11">
         <v>1904</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="A22" s="11">
         <v>1905</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="A23" s="11">
         <v>1906</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="A24" s="11">
         <v>1907</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="A25" s="11">
         <v>1908</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="A26" s="11">
         <v>1909</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="A27" s="11">
         <v>1910</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="A28" s="11">
         <v>1911</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="A29" s="11">
         <v>1912</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30">
+      <c r="A30" s="11">
         <v>1913</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="A31" s="11">
         <v>1914</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32">
+      <c r="A32" s="11">
         <v>1915</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="A33" s="11">
         <v>1916</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="A34" s="11">
         <v>1917</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="A35" s="11">
         <v>1918</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36">
+      <c r="A36" s="11">
         <v>1919</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37">
+      <c r="A37" s="11">
         <v>1920</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38">
+      <c r="A38" s="11">
         <v>1921</v>
       </c>
     </row>
     <row r="39" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39">
+      <c r="A39" s="11">
         <v>1922</v>
       </c>
     </row>
     <row r="40" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40">
+      <c r="A40" s="11">
         <v>1923</v>
       </c>
     </row>
     <row r="41" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41">
+      <c r="A41" s="11">
         <v>1924</v>
       </c>
     </row>
     <row r="42" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42">
+      <c r="A42" s="11">
         <v>1925</v>
       </c>
     </row>
     <row r="43" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43">
+      <c r="A43" s="11">
         <v>1926</v>
       </c>
     </row>
     <row r="44" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44">
+      <c r="A44" s="11">
         <v>1927</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45">
+      <c r="A45" s="11">
         <v>1928</v>
       </c>
     </row>
     <row r="46" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46">
+      <c r="A46" s="11">
         <v>1929</v>
       </c>
     </row>
     <row r="47" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47">
+      <c r="A47" s="11">
         <v>1930</v>
       </c>
     </row>
     <row r="48" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48">
+      <c r="A48" s="11">
         <v>1931</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49">
+      <c r="A49" s="11">
         <v>1932</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50">
+      <c r="A50" s="11">
         <v>1933</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51">
+      <c r="A51" s="11">
         <v>1934</v>
       </c>
     </row>
     <row r="52" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52">
+      <c r="A52" s="11">
         <v>1935</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53">
+      <c r="A53" s="11">
         <v>1936</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54">
+      <c r="A54" s="11">
         <v>1937</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55">
+      <c r="A55" s="11">
         <v>1938</v>
       </c>
     </row>
     <row r="56" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56">
+      <c r="A56" s="11">
         <v>1939</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57">
+      <c r="A57" s="11">
         <v>1940</v>
       </c>
     </row>
     <row r="58" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58">
+      <c r="A58" s="11">
         <v>1941</v>
       </c>
     </row>
     <row r="59" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59">
+      <c r="A59" s="11">
         <v>1942</v>
       </c>
     </row>
     <row r="60" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60">
+      <c r="A60" s="11">
         <v>1943</v>
       </c>
     </row>
     <row r="61" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61">
+      <c r="A61" s="11">
         <v>1944</v>
       </c>
     </row>
     <row r="62" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62">
+      <c r="A62" s="11">
         <v>1945</v>
       </c>
     </row>
     <row r="63" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63">
+      <c r="A63" s="11">
         <v>1946</v>
       </c>
     </row>
     <row r="64" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64">
+      <c r="A64" s="11">
         <v>1947</v>
       </c>
     </row>
     <row r="65" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65">
+      <c r="A65" s="11">
         <v>1948</v>
       </c>
     </row>
     <row r="66" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66">
+      <c r="A66" s="11">
         <v>1949</v>
       </c>
     </row>
     <row r="67" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67">
+      <c r="A67" s="11">
         <v>1950</v>
       </c>
     </row>
     <row r="68" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68">
+      <c r="A68" s="11">
         <v>1951</v>
       </c>
     </row>
     <row r="69" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69">
+      <c r="A69" s="11">
         <v>1952</v>
       </c>
     </row>
     <row r="70" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70">
+      <c r="A70" s="11">
         <v>1953</v>
       </c>
     </row>
     <row r="71" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71">
+      <c r="A71" s="11">
         <v>1954</v>
       </c>
     </row>
     <row r="72" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72">
+      <c r="A72" s="11">
         <v>1955</v>
       </c>
     </row>
     <row r="73" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73">
+      <c r="A73" s="11">
         <v>1956</v>
       </c>
     </row>
     <row r="74" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74">
+      <c r="A74" s="11">
         <v>1957</v>
       </c>
     </row>
     <row r="75" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75">
+      <c r="A75" s="11">
         <v>1958</v>
       </c>
     </row>
     <row r="76" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76">
+      <c r="A76" s="11">
         <v>1959</v>
       </c>
     </row>
     <row r="77" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77">
+      <c r="A77" s="11">
         <v>1960</v>
       </c>
     </row>
     <row r="78" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78">
+      <c r="A78" s="11">
         <v>1961</v>
       </c>
     </row>
     <row r="79" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79">
+      <c r="A79" s="11">
         <v>1962</v>
       </c>
     </row>
     <row r="80" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80">
+      <c r="A80" s="11">
         <v>1963</v>
       </c>
     </row>
     <row r="81" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81">
+      <c r="A81" s="11">
         <v>1964</v>
       </c>
     </row>
     <row r="82" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82">
+      <c r="A82" s="11">
         <v>1965</v>
       </c>
     </row>
     <row r="83" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83">
+      <c r="A83" s="11">
         <v>1966</v>
       </c>
     </row>
     <row r="84" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84">
+      <c r="A84" s="11">
         <v>1967</v>
       </c>
     </row>
     <row r="85" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85">
+      <c r="A85" s="11">
         <v>1968</v>
       </c>
     </row>
     <row r="86" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86">
+      <c r="A86" s="11">
         <v>1969</v>
       </c>
     </row>
     <row r="87" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87">
+      <c r="A87" s="11">
         <v>1970</v>
       </c>
     </row>
     <row r="88" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88">
+      <c r="A88" s="11">
         <v>1971</v>
       </c>
     </row>
     <row r="89" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89">
+      <c r="A89" s="11">
         <v>1972</v>
       </c>
     </row>
     <row r="90" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90">
+      <c r="A90" s="11">
         <v>1973</v>
       </c>
     </row>
     <row r="91" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91">
+      <c r="A91" s="11">
         <v>1974</v>
       </c>
     </row>
     <row r="92" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92">
+      <c r="A92" s="11">
         <v>1975</v>
       </c>
     </row>
     <row r="93" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93">
+      <c r="A93" s="11">
         <v>1976</v>
       </c>
     </row>
     <row r="94" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94">
+      <c r="A94" s="11">
         <v>1977</v>
       </c>
     </row>
     <row r="95" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95">
+      <c r="A95" s="11">
         <v>1978</v>
       </c>
     </row>
     <row r="96" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96">
+      <c r="A96" s="11">
         <v>1979</v>
       </c>
     </row>
     <row r="97" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97">
+      <c r="A97" s="11">
         <v>1980</v>
       </c>
     </row>
     <row r="98" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98">
+      <c r="A98" s="11">
         <v>1981</v>
       </c>
     </row>
     <row r="99" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99">
+      <c r="A99" s="11">
         <v>1982</v>
       </c>
     </row>
     <row r="100" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100">
+      <c r="A100" s="11">
         <v>1983</v>
       </c>
     </row>
     <row r="101" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101">
+      <c r="A101" s="11">
         <v>1984</v>
       </c>
     </row>
     <row r="102" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102">
+      <c r="A102" s="11">
         <v>1985</v>
       </c>
     </row>
     <row r="103" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103">
+      <c r="A103" s="11">
         <v>1986</v>
       </c>
     </row>
     <row r="104" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104">
+      <c r="A104" s="11">
         <v>1987</v>
       </c>
     </row>
     <row r="105" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105">
+      <c r="A105" s="11">
         <v>1988</v>
       </c>
     </row>
     <row r="106" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106">
+      <c r="A106" s="11">
         <v>1989</v>
       </c>
     </row>
     <row r="107" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107">
+      <c r="A107" s="11">
         <v>1990</v>
       </c>
     </row>
     <row r="108" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108">
+      <c r="A108" s="11">
         <v>1991</v>
       </c>
     </row>
     <row r="109" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109">
+      <c r="A109" s="11">
         <v>1992</v>
       </c>
     </row>
     <row r="110" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110">
+      <c r="A110" s="11">
         <v>1993</v>
       </c>
     </row>
     <row r="111" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111">
+      <c r="A111" s="11">
         <v>1994</v>
       </c>
     </row>
     <row r="112" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112">
+      <c r="A112" s="11">
         <v>1995</v>
       </c>
     </row>
     <row r="113" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113">
+      <c r="A113" s="11">
         <v>1996</v>
       </c>
     </row>
     <row r="114" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114">
+      <c r="A114" s="11">
         <v>1997</v>
       </c>
     </row>
     <row r="115" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115">
+      <c r="A115" s="11">
         <v>1998</v>
       </c>
     </row>
     <row r="116" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116">
+      <c r="A116" s="11">
         <v>1999</v>
       </c>
     </row>
     <row r="117" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117">
+      <c r="A117" s="11">
         <v>2000</v>
       </c>
     </row>
     <row r="118" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118">
+      <c r="A118" s="11">
         <v>2001</v>
       </c>
     </row>
     <row r="119" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119">
+      <c r="A119" s="11">
         <v>2002</v>
       </c>
     </row>
     <row r="120" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120">
+      <c r="A120" s="11">
         <v>2003</v>
       </c>
     </row>
     <row r="121" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121">
+      <c r="A121" s="11">
         <v>2004</v>
       </c>
     </row>
     <row r="122" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122">
+      <c r="A122" s="11">
         <v>2005</v>
       </c>
     </row>
     <row r="123" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123">
+      <c r="A123" s="11">
         <v>2006</v>
       </c>
     </row>
     <row r="124" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124">
+      <c r="A124" s="11">
         <v>2007</v>
       </c>
     </row>
     <row r="125" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125">
+      <c r="A125" s="11">
         <v>2008</v>
       </c>
     </row>
     <row r="126" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126">
+      <c r="A126" s="11">
         <v>2009</v>
       </c>
     </row>
     <row r="127" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127">
+      <c r="A127" s="11">
         <v>2010</v>
       </c>
     </row>
     <row r="128" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128">
+      <c r="A128" s="11">
         <v>2011</v>
       </c>
     </row>
     <row r="129" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129">
+      <c r="A129" s="11">
         <v>2012</v>
       </c>
     </row>
     <row r="130" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130">
+      <c r="A130" s="11">
         <v>2013</v>
       </c>
     </row>
     <row r="131" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131">
+      <c r="A131" s="11">
         <v>2014</v>
       </c>
     </row>
     <row r="132" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132">
+      <c r="A132" s="11">
         <v>2015</v>
       </c>
     </row>
     <row r="133" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133">
+      <c r="A133" s="11">
         <v>2016</v>
       </c>
     </row>
     <row r="134" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134">
+      <c r="A134" s="11">
         <v>2017</v>
       </c>
     </row>
     <row r="135" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135">
+      <c r="A135" s="11">
         <v>2018</v>
       </c>
     </row>
     <row r="136" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136">
+      <c r="A136" s="11">
         <v>2019</v>
       </c>
     </row>
     <row r="137" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137">
+      <c r="A137" s="11">
         <v>2020</v>
       </c>
     </row>
     <row r="138" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138">
+      <c r="A138" s="11">
         <v>2021</v>
       </c>
     </row>
     <row r="139" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139">
+      <c r="A139" s="11">
         <v>2022</v>
       </c>
     </row>
     <row r="140" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A140">
+      <c r="A140" s="11">
         <v>2023</v>
       </c>
     </row>
     <row r="141" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141">
+      <c r="A141" s="11">
         <v>2024</v>
       </c>
     </row>
     <row r="142" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A142">
+      <c r="A142" s="11">
         <v>2025</v>
       </c>
     </row>
     <row r="143" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143">
+      <c r="A143" s="11">
         <v>2026</v>
       </c>
     </row>
     <row r="144" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A144">
+      <c r="A144" s="11">
         <v>2027</v>
       </c>
     </row>
     <row r="145" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A145">
+      <c r="A145" s="11">
         <v>2028</v>
       </c>
     </row>
     <row r="146" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A146">
+      <c r="A146" s="11">
         <v>2029</v>
       </c>
     </row>
     <row r="147" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A147">
+      <c r="A147" s="11">
         <v>2030</v>
       </c>
     </row>
     <row r="148" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A148">
+      <c r="A148" s="11">
         <v>2031</v>
       </c>
     </row>
     <row r="149" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A149">
+      <c r="A149" s="11">
         <v>2032</v>
       </c>
     </row>
     <row r="150" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A150">
+      <c r="A150" s="11">
         <v>2033</v>
       </c>
     </row>
     <row r="151" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A151">
+      <c r="A151" s="11">
         <v>2034</v>
       </c>
     </row>
     <row r="152" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A152">
+      <c r="A152" s="11">
         <v>2035</v>
       </c>
     </row>
     <row r="153" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A153">
+      <c r="A153" s="11">
         <v>2036</v>
       </c>
     </row>
     <row r="154" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A154">
+      <c r="A154" s="11">
         <v>2037</v>
       </c>
     </row>
     <row r="155" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A155">
+      <c r="A155" s="11">
         <v>2038</v>
       </c>
     </row>
     <row r="156" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A156">
+      <c r="A156" s="11">
         <v>2039</v>
       </c>
     </row>
     <row r="157" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A157">
+      <c r="A157" s="11">
         <v>2040</v>
       </c>
     </row>
     <row r="158" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A158">
+      <c r="A158" s="11">
         <v>2041</v>
       </c>
     </row>
     <row r="159" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A159">
+      <c r="A159" s="11">
         <v>2042</v>
       </c>
     </row>
     <row r="160" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A160">
+      <c r="A160" s="11">
         <v>2043</v>
       </c>
     </row>
     <row r="161" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A161">
+      <c r="A161" s="11">
         <v>2044</v>
       </c>
     </row>
     <row r="162" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A162">
+      <c r="A162" s="11">
         <v>2045</v>
       </c>
     </row>
     <row r="163" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A163">
+      <c r="A163" s="11">
         <v>2046</v>
       </c>
     </row>
     <row r="164" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A164">
+      <c r="A164" s="11">
         <v>2047</v>
       </c>
     </row>
     <row r="165" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A165">
+      <c r="A165" s="11">
         <v>2048</v>
       </c>
     </row>
     <row r="166" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A166">
+      <c r="A166" s="11">
         <v>2049</v>
       </c>
     </row>
     <row r="167" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A167">
+      <c r="A167" s="11">
         <v>2050</v>
       </c>
     </row>
     <row r="168" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A168">
+      <c r="A168" s="11">
         <v>2051</v>
       </c>
     </row>
     <row r="169" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A169">
+      <c r="A169" s="11">
         <v>2052</v>
       </c>
     </row>
     <row r="170" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A170">
+      <c r="A170" s="11">
         <v>2053</v>
       </c>
     </row>
     <row r="171" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A171">
+      <c r="A171" s="11">
         <v>2054</v>
       </c>
     </row>
     <row r="172" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A172">
+      <c r="A172" s="11">
         <v>2055</v>
       </c>
     </row>
     <row r="173" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A173">
+      <c r="A173" s="11">
         <v>2056</v>
       </c>
     </row>
     <row r="174" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A174">
+      <c r="A174" s="11">
         <v>2057</v>
       </c>
     </row>
     <row r="175" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A175">
+      <c r="A175" s="11">
         <v>2058</v>
       </c>
     </row>
     <row r="176" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A176">
+      <c r="A176" s="11">
         <v>2059</v>
       </c>
     </row>
     <row r="177" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A177">
+      <c r="A177" s="11">
         <v>2060</v>
       </c>
     </row>
     <row r="178" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A178">
+      <c r="A178" s="11">
         <v>2061</v>
       </c>
     </row>
     <row r="179" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A179">
+      <c r="A179" s="11">
         <v>2062</v>
       </c>
     </row>
     <row r="180" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A180">
+      <c r="A180" s="11">
         <v>2063</v>
       </c>
     </row>
     <row r="181" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A181">
+      <c r="A181" s="11">
         <v>2064</v>
       </c>
     </row>
     <row r="182" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A182">
+      <c r="A182" s="11">
         <v>2065</v>
       </c>
     </row>
     <row r="183" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A183">
+      <c r="A183" s="11">
         <v>2066</v>
       </c>
     </row>
     <row r="184" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A184">
+      <c r="A184" s="11">
         <v>2067</v>
       </c>
     </row>
     <row r="185" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A185">
+      <c r="A185" s="11">
         <v>2068</v>
       </c>
     </row>
     <row r="186" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A186">
+      <c r="A186" s="11">
         <v>2069</v>
       </c>
     </row>
     <row r="187" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A187">
+      <c r="A187" s="11">
         <v>2070</v>
       </c>
     </row>
     <row r="188" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A188">
+      <c r="A188" s="11">
         <v>2071</v>
       </c>
     </row>
     <row r="189" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A189">
+      <c r="A189" s="11">
         <v>2072</v>
       </c>
     </row>
     <row r="190" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A190">
+      <c r="A190" s="11">
         <v>2073</v>
       </c>
     </row>
     <row r="191" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A191">
+      <c r="A191" s="11">
         <v>2074</v>
       </c>
     </row>
     <row r="192" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A192">
+      <c r="A192" s="11">
         <v>2075</v>
       </c>
     </row>
     <row r="193" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A193">
+      <c r="A193" s="11">
         <v>2076</v>
       </c>
     </row>
     <row r="194" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A194">
+      <c r="A194" s="11">
         <v>2077</v>
       </c>
     </row>
     <row r="195" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A195">
+      <c r="A195" s="11">
         <v>2078</v>
       </c>
     </row>
     <row r="196" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A196">
+      <c r="A196" s="11">
         <v>2079</v>
       </c>
     </row>
     <row r="197" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A197">
+      <c r="A197" s="11">
         <v>2080</v>
       </c>
     </row>
     <row r="198" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A198">
+      <c r="A198" s="11">
         <v>2081</v>
       </c>
     </row>
     <row r="199" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A199">
+      <c r="A199" s="11">
         <v>2082</v>
       </c>
     </row>
     <row r="200" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A200">
+      <c r="A200" s="11">
         <v>2083</v>
       </c>
     </row>
     <row r="201" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A201">
+      <c r="A201" s="11">
         <v>2084</v>
       </c>
     </row>
     <row r="202" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A202">
+      <c r="A202" s="11">
         <v>2085</v>
       </c>
     </row>
     <row r="203" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A203">
+      <c r="A203" s="11">
         <v>2086</v>
       </c>
     </row>
     <row r="204" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A204">
+      <c r="A204" s="11">
         <v>2087</v>
       </c>
     </row>
     <row r="205" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A205">
+      <c r="A205" s="11">
         <v>2088</v>
       </c>
     </row>
     <row r="206" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A206">
+      <c r="A206" s="11">
         <v>2089</v>
       </c>
     </row>
     <row r="207" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A207">
+      <c r="A207" s="11">
         <v>2090</v>
       </c>
     </row>
     <row r="208" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A208">
+      <c r="A208" s="11">
         <v>2091</v>
       </c>
     </row>
     <row r="209" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A209">
+      <c r="A209" s="11">
         <v>2092</v>
       </c>
     </row>
     <row r="210" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A210">
+      <c r="A210" s="11">
         <v>2093</v>
       </c>
     </row>
     <row r="211" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A211">
+      <c r="A211" s="11">
         <v>2094</v>
       </c>
     </row>
     <row r="212" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A212">
+      <c r="A212" s="11">
         <v>2095</v>
       </c>
     </row>
     <row r="213" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A213">
+      <c r="A213" s="11">
         <v>2096</v>
       </c>
     </row>
     <row r="214" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A214">
+      <c r="A214" s="11">
         <v>2097</v>
       </c>
     </row>
     <row r="215" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A215">
+      <c r="A215" s="11">
         <v>2098</v>
       </c>
     </row>
     <row r="216" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A216">
+      <c r="A216" s="11">
         <v>2099</v>
       </c>
     </row>
     <row r="217" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A217">
+      <c r="A217" s="11">
         <v>2100</v>
       </c>
     </row>
@@ -3433,6 +3451,10 @@
     <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <protectedRanges>
+    <protectedRange algorithmName="SHA-512" hashValue="/q8Ok7typBGb7piMMz3p00gp+srVmcJlldS7VJ77JC/8n46jfs3MSKmeb3Qdb6/s7n0ZUxjFmRe+g7a0KuW/Rw==" saltValue="DYSPSKOzgREouIEEc8u+Ig==" spinCount="100000" sqref="A1:A217 C1:I10" name="Intervalo1"/>
+  </protectedRanges>
   <mergeCells count="4">
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="E3:G3"/>

</xml_diff>